<commit_message>
Bổ sung quyết định giao lại đất trong báo cáo
</commit_message>
<xml_diff>
--- a/QuanLyThueDat.WebApp/Assets/Template/MauBaoCaoDoanhNghiepThueDat.xlsx
+++ b/QuanLyThueDat.WebApp/Assets/Template/MauBaoCaoDoanhNghiepThueDat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNPT\QuanLyThueDat\QuanLyThueDat\QuanLyThueDat.WebApp\Assets\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7F47D4-DD3B-4A2F-A338-26E24A0B9992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF782DED-784F-497A-A1F0-1DF0ED9533E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>UBND TỈNH NGHỆ AN</t>
   </si>
@@ -107,6 +107,21 @@
   </si>
   <si>
     <t>Ngày thông báo</t>
+  </si>
+  <si>
+    <t>Quyết định giao lại đất</t>
+  </si>
+  <si>
+    <t>Số QĐ ngày tháng</t>
+  </si>
+  <si>
+    <t>Giao đất có thu tiền m2</t>
+  </si>
+  <si>
+    <t>Giao đất không thu tiền m2</t>
+  </si>
+  <si>
+    <t>Tổng cộng</t>
   </si>
 </sst>
 </file>
@@ -266,7 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -295,12 +310,24 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -322,16 +349,13 @@
     <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -615,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,66 +652,76 @@
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="7" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="6" max="12" width="18.5703125" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="2"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="3"/>
       <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
     </row>
-    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="2"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="3"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
     </row>
-    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -695,164 +729,197 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="2"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="3"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="17"/>
+      <c r="AA3" s="17"/>
     </row>
-    <row r="4" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16"/>
     </row>
-    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="11" t="s">
+      <c r="G5" s="22"/>
+      <c r="H5" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="20" t="s">
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="11" t="s">
+      <c r="U5" s="14"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="10" t="s">
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="19" t="s">
+    <row r="6" spans="1:27" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="10" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="O6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="P6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="Q6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="R6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="T6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="U6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="V6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="W6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="S6" s="5" t="s">
+      <c r="X6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="T6" s="6" t="s">
+      <c r="Y6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="U6" s="5" t="s">
+      <c r="Z6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="V6" s="10"/>
+      <c r="AA6" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="A4:V4"/>
-    <mergeCell ref="R1:V3"/>
+  <mergeCells count="15">
+    <mergeCell ref="AA5:AA6"/>
+    <mergeCell ref="W5:Z5"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="A4:AA4"/>
+    <mergeCell ref="W1:AA3"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="H5:N5"/>
+    <mergeCell ref="M5:S5"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>